<commit_message>
Fix docs, typos, excel parsing and parsing test
</commit_message>
<xml_diff>
--- a/Lab1_creditPay/app/src/main/resources/excel/exampleData.xlsx
+++ b/Lab1_creditPay/app/src/main/resources/excel/exampleData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Дата платежа</t>
   </si>
   <si>
-    <t xml:space="preserve">Дата предоставление кредита</t>
+    <t xml:space="preserve">Дата предоставления кредита</t>
   </si>
   <si>
     <t xml:space="preserve">22.09.2022</t>
@@ -72,7 +72,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -125,11 +124,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -322,10 +321,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -336,116 +335,53 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="2" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="G1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="1" t="n">
         <v>9200000</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="1" t="n">
         <v>276</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="1" t="n">
         <v>7.45</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>